<commit_message>
Cleaning up, commenting, fix sound sample format
</commit_message>
<xml_diff>
--- a/docs/555 workings.xlsx
+++ b/docs/555 workings.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\Arcade-Blockade_MiSTer\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{088FD943-11C2-44BE-8557-E1F786604743}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDEAA2D0-BE5C-4765-99C5-124344110581}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1125" yWindow="2565" windowWidth="24165" windowHeight="14085" xr2:uid="{2689206F-860B-425A-BE78-CA48063DCFFF}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{2689206F-860B-425A-BE78-CA48063DCFFF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
     <definedName name="CAPSCALE">Sheet1!$G$6</definedName>
+    <definedName name="SYS_CLOCK">Sheet1!$G$18</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -429,7 +430,7 @@
   <dimension ref="B1:P21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -535,8 +536,12 @@
         <v>93681.5</v>
       </c>
       <c r="I10">
-        <f>G18/H10</f>
+        <f>SYS_CLOCK/H10</f>
         <v>221.92215111841719</v>
+      </c>
+      <c r="J10">
+        <f>SYS_CLOCK/H10/2</f>
+        <v>110.9610755592086</v>
       </c>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.25">
@@ -558,6 +563,10 @@
         <f>I10/F11*D10</f>
         <v>140.95055544007579</v>
       </c>
+      <c r="J11">
+        <f>J10/F11*D10</f>
+        <v>70.475277720037894</v>
+      </c>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
@@ -573,6 +582,10 @@
       <c r="I12">
         <f>I11/F11*D11</f>
         <v>51.427905363270895</v>
+      </c>
+      <c r="J12">
+        <f>J11/F11*D11</f>
+        <v>25.713952681635448</v>
       </c>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.25">

</xml_diff>